<commit_message>
adapted Analysis on final UK data
</commit_message>
<xml_diff>
--- a/08_UK_Data/02_Output/TRI_Components_Means.xlsx
+++ b/08_UK_Data/02_Output/TRI_Components_Means.xlsx
@@ -377,7 +377,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>4.80</t>
+          <t>4.78</t>
         </is>
       </c>
     </row>
@@ -389,7 +389,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>3.51</t>
+          <t>3.49</t>
         </is>
       </c>
     </row>
@@ -401,7 +401,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>3.51</t>
+          <t>3.52</t>
         </is>
       </c>
     </row>
@@ -413,7 +413,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>3.88</t>
+          <t>3.89</t>
         </is>
       </c>
     </row>
@@ -425,7 +425,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>4.23</t>
+          <t>4.22</t>
         </is>
       </c>
     </row>

</xml_diff>